<commit_message>
thurst data 9th Jan
</commit_message>
<xml_diff>
--- a/Datadump/Thrust Bench/Motor Burn Test - 3/Calculation for Test.xlsx
+++ b/Datadump/Thrust Bench/Motor Burn Test - 3/Calculation for Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikhil\Documents\GitHub\Tejas-Flight-Computer\Datadump\Thrust Bench\Motor Burn Test - 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E64ACA6E-F8BE-4D40-8F45-0FD7D35B5392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B96ED1-8838-4AB7-A4E4-C52466DE734F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AFAB93E4-75EF-4035-B3DF-7924F1D6ABB5}"/>
   </bookViews>
@@ -116,10 +116,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +437,7 @@
   <dimension ref="B1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,10 +653,10 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="3"/>
       <c r="E16">
         <f>D14*E14</f>
         <v>0.5666944666666669</v>
@@ -670,10 +670,10 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="3"/>
       <c r="E18">
         <f>F16/0.045</f>
         <v>123.41346162962969</v>
@@ -683,15 +683,15 @@
       </c>
     </row>
     <row r="20" spans="3:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="3"/>
       <c r="E20">
         <f>F16/C14</f>
         <v>9.675271382113813</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>